<commit_message>
Blocked Camera in Intro and Congrats
</commit_message>
<xml_diff>
--- a/ExcelTasks/TasksExcel.xlsx
+++ b/ExcelTasks/TasksExcel.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanha2\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Tasks</t>
   </si>
@@ -48,12 +43,24 @@
   </si>
   <si>
     <t>Juan Hernández</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blocking Camera </t>
+  </si>
+  <si>
+    <t>Xavier Trillo</t>
+  </si>
+  <si>
+    <t>0 hours and 15 minutes</t>
+  </si>
+  <si>
+    <t>0 hours and 30 minutes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -178,7 +185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -213,7 +220,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -390,7 +397,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -398,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:E8"/>
+  <dimension ref="B5:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,6 +450,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Smoth Mecanics With Collision Hitboxes
</commit_message>
<xml_diff>
--- a/ExcelTasks/TasksExcel.xlsx
+++ b/ExcelTasks/TasksExcel.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martitg\Documents\GitHub\Arial--Comic-Sans--Dealers\ExcelTasks\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="13740"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Tasks</t>
   </si>
@@ -66,12 +61,27 @@
   </si>
   <si>
     <t>1 week aproximately ( day up, day down)</t>
+  </si>
+  <si>
+    <t>Basic Movement</t>
+  </si>
+  <si>
+    <t>1 hour and 30 minutes</t>
+  </si>
+  <si>
+    <t>Smoth Animations</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>Collision Boxes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -408,7 +418,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -416,21 +426,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:E9"/>
+  <dimension ref="B5:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.88671875" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="2:5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="1" t="s">
         <v>0</v>
@@ -445,7 +455,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -453,7 +463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -467,7 +477,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -478,6 +488,48 @@
         <v>10</v>
       </c>
       <c r="E9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Forward and Backward Jump
</commit_message>
<xml_diff>
--- a/ExcelTasks/TasksExcel.xlsx
+++ b/ExcelTasks/TasksExcel.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adri\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E40513-C9A6-4312-869E-ECCA89B9DF31}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Tasks</t>
   </si>
@@ -103,12 +97,24 @@
   </si>
   <si>
     <t>30 minutes</t>
+  </si>
+  <si>
+    <t>Back and Forw Jump</t>
+  </si>
+  <si>
+    <t>Neutral Jump Smooth</t>
+  </si>
+  <si>
+    <t>0 hours and 45 minutes</t>
+  </si>
+  <si>
+    <t>1 hour and 45 minutes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -445,18 +451,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B5:E15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,6 +608,34 @@
         <v>21</v>
       </c>
     </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added font module and counter with font module
</commit_message>
<xml_diff>
--- a/ExcelTasks/TasksExcel.xlsx
+++ b/ExcelTasks/TasksExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\Arial--Comic-Sans--Dealers\ExcelTasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBF7353-19FA-4F01-8E58-82027DD5C824}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06370D7D-25BE-454C-BF74-DAC2B224D37F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="48">
   <si>
     <t>Tasks</t>
   </si>
@@ -144,9 +144,6 @@
     <t>2hours</t>
   </si>
   <si>
-    <t>Updated Camera movement and reset</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fixed neutral punch jump animation </t>
   </si>
   <si>
@@ -160,6 +157,18 @@
   </si>
   <si>
     <t xml:space="preserve">Added damage </t>
+  </si>
+  <si>
+    <t>Updated Camera movement and reset camera</t>
+  </si>
+  <si>
+    <t>Death animation</t>
+  </si>
+  <si>
+    <t>4 hours</t>
+  </si>
+  <si>
+    <t>Round points</t>
   </si>
 </sst>
 </file>
@@ -510,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B5:E28"/>
+  <dimension ref="B5:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="I18" sqref="I18:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +643,7 @@
         <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -779,7 +788,7 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
@@ -793,7 +802,7 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
@@ -802,12 +811,12 @@
         <v>23</v>
       </c>
       <c r="E25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
@@ -821,7 +830,7 @@
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
@@ -835,7 +844,7 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -845,6 +854,34 @@
       </c>
       <c r="E28" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sound Efects and Score Player 1
</commit_message>
<xml_diff>
--- a/ExcelTasks/TasksExcel.xlsx
+++ b/ExcelTasks/TasksExcel.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adri\Documents\GitHub\Arial--Comic-Sans--Dealers\ExcelTasks\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8968EC-B513-46F2-93D5-8B377B20FA3D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="82">
   <si>
     <t>Tasks</t>
   </si>
@@ -219,15 +213,9 @@
     <t>14 hours</t>
   </si>
   <si>
-    <t>8,5 hours</t>
-  </si>
-  <si>
     <t>27 hours</t>
   </si>
   <si>
-    <t>13 hours</t>
-  </si>
-  <si>
     <t>3 hour</t>
   </si>
   <si>
@@ -262,13 +250,28 @@
   </si>
   <si>
     <t>20 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dalshim Stage </t>
+  </si>
+  <si>
+    <t>Title Screen and Character Selection Sound Effects</t>
+  </si>
+  <si>
+    <t>2 houts</t>
+  </si>
+  <si>
+    <t>10 hours</t>
+  </si>
+  <si>
+    <t>19 hours</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,7 +383,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -651,32 +654,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B5:I44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B5:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="46.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="46.36328125" customWidth="1"/>
+    <col min="3" max="3" width="23.54296875" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="38.6640625" customWidth="1"/>
+    <col min="5" max="5" width="38.6328125" customWidth="1"/>
     <col min="8" max="8" width="26" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="9" max="9" width="22.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="2:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:9" ht="15" thickBot="1"/>
+    <row r="6" spans="2:9" ht="18" customHeight="1" thickBot="1">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
@@ -696,7 +699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -716,10 +719,10 @@
         <v>62</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
       <c r="B8" t="s">
         <v>22</v>
       </c>
@@ -739,10 +742,10 @@
         <v>63</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
       <c r="B9" t="s">
         <v>28</v>
       </c>
@@ -759,15 +762,15 @@
         <v>48</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
       <c r="B10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>19</v>
@@ -782,15 +785,15 @@
         <v>49</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
       <c r="B11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>19</v>
@@ -802,9 +805,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9">
       <c r="B12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>19</v>
@@ -816,9 +819,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9">
       <c r="B13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>19</v>
@@ -830,9 +833,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9">
       <c r="B14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>19</v>
@@ -844,9 +847,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9">
       <c r="B15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>19</v>
@@ -858,9 +861,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9">
       <c r="B16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>19</v>
@@ -872,7 +875,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="B17" t="s">
         <v>8</v>
       </c>
@@ -886,7 +889,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="B18" t="s">
         <v>13</v>
       </c>
@@ -900,7 +903,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5">
       <c r="B19" t="s">
         <v>15</v>
       </c>
@@ -914,7 +917,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5">
       <c r="B20" t="s">
         <v>17</v>
       </c>
@@ -928,7 +931,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5">
       <c r="B21" t="s">
         <v>25</v>
       </c>
@@ -942,7 +945,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5">
       <c r="B22" t="s">
         <v>24</v>
       </c>
@@ -956,51 +959,51 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5">
       <c r="B23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" t="s">
         <v>4</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>42</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
       <c r="B26" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>7</v>
@@ -1009,110 +1012,110 @@
         <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
       <c r="B27" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
       <c r="B28" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
       <c r="B29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D29" t="s">
-        <v>57</v>
+      <c r="D29" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
       <c r="B30" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" t="s">
         <v>16</v>
       </c>
-      <c r="E30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="2:5">
       <c r="B31" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E33" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
+    <row r="34" spans="2:5">
+      <c r="B34" t="s">
         <v>5</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
-        <v>31</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>6</v>
@@ -1121,146 +1124,174 @@
         <v>20</v>
       </c>
       <c r="E34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5">
       <c r="B35" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5">
       <c r="B36" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5">
       <c r="B37" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E37" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5">
       <c r="B38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E38" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5">
       <c r="B39" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="E39" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5">
       <c r="B40" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E40" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5">
       <c r="B41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E41" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5">
       <c r="B42" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E42" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5">
       <c r="B43" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E43" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5">
       <c r="B44" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="B45" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5">
+      <c r="B46" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E46" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Score And Sound Effects Finished
</commit_message>
<xml_diff>
--- a/ExcelTasks/TasksExcel.xlsx
+++ b/ExcelTasks/TasksExcel.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUCERO\Desktop\Arial--Comic-Sans--Dealers\ExcelTasks\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="11025"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="84">
   <si>
     <t>Tasks</t>
   </si>
@@ -51,9 +56,6 @@
     <t>Xavier Trillo</t>
   </si>
   <si>
-    <t>0 hours and 15 minutes</t>
-  </si>
-  <si>
     <t>0 hours and 30 minutes</t>
   </si>
   <si>
@@ -255,23 +257,32 @@
     <t xml:space="preserve">Dalshim Stage </t>
   </si>
   <si>
-    <t>Title Screen and Character Selection Sound Effects</t>
-  </si>
-  <si>
     <t>2 houts</t>
   </si>
   <si>
     <t>10 hours</t>
   </si>
   <si>
-    <t>19 hours</t>
+    <t>Title Screen and Character Selection Sounds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 hours </t>
+  </si>
+  <si>
+    <t>Player 1 Score Fixes And Sound Effects</t>
+  </si>
+  <si>
+    <t>Player 2 Score Fixes And Sound Efects</t>
+  </si>
+  <si>
+    <t>21,5 hours</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,7 +394,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Buena" xfId="1" builtinId="26"/>
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -654,32 +665,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B5:I46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="46.36328125" customWidth="1"/>
-    <col min="3" max="3" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="38.6328125" customWidth="1"/>
+    <col min="5" max="5" width="38.5703125" customWidth="1"/>
     <col min="8" max="8" width="26" customWidth="1"/>
-    <col min="9" max="9" width="22.36328125" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:9" ht="15" thickBot="1"/>
-    <row r="6" spans="2:9" ht="18" customHeight="1" thickBot="1">
+    <row r="5" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,189 +704,189 @@
         <v>3</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9">
-      <c r="B8" t="s">
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="E12" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" t="s">
-        <v>47</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9">
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="8" t="s">
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9">
-      <c r="B10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="8" t="s">
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9">
-      <c r="B11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="8" t="s">
+      <c r="E16" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9">
-      <c r="B12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9">
-      <c r="B13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9">
-      <c r="B14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9">
-      <c r="B15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9">
-      <c r="B16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>8</v>
       </c>
@@ -886,413 +897,441 @@
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>14</v>
-      </c>
-      <c r="E18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" t="s">
-        <v>15</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" t="s">
-        <v>17</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>4</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5">
-      <c r="B26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5">
-      <c r="B27" t="s">
-        <v>42</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E29" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E30" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D31" t="s">
-        <v>57</v>
+      <c r="D31" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="E31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>20</v>
+      <c r="D33" t="s">
+        <v>56</v>
       </c>
       <c r="E33" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>5</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5">
-      <c r="B35" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="B36" t="s">
-        <v>31</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="E37" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E38" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E39" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="E41" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E42" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E43" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E44" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E45" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E46" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>